<commit_message>
Transform excel parsing data to json objects
</commit_message>
<xml_diff>
--- a/src/resources/TestData.xlsx
+++ b/src/resources/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Old ID</t>
   </si>
@@ -63,18 +63,6 @@
     <t>body</t>
   </si>
   <si>
-    <t>Plastname</t>
-  </si>
-  <si>
-    <t>Psurname</t>
-  </si>
-  <si>
-    <t>Pbirthday</t>
-  </si>
-  <si>
-    <t>Pplz</t>
-  </si>
-  <si>
     <t>Input</t>
   </si>
   <si>
@@ -84,9 +72,6 @@
     <t>Post Comment</t>
   </si>
   <si>
-    <t>Lorem Ipsun</t>
-  </si>
-  <si>
     <t>Max</t>
   </si>
   <si>
@@ -109,6 +94,51 @@
   </si>
   <si>
     <t>TC-2</t>
+  </si>
+  <si>
+    <t>Perssurname</t>
+  </si>
+  <si>
+    <t>Perslastname</t>
+  </si>
+  <si>
+    <t>Persbirthdate</t>
+  </si>
+  <si>
+    <t>Persplz</t>
+  </si>
+  <si>
+    <t>TC-3</t>
+  </si>
+  <si>
+    <t>Input-Add</t>
+  </si>
+  <si>
+    <t>Result-Add</t>
+  </si>
+  <si>
+    <t>Test TC-3</t>
+  </si>
+  <si>
+    <t>Test one</t>
+  </si>
+  <si>
+    <t>Test three</t>
+  </si>
+  <si>
+    <t>Emiliy</t>
+  </si>
+  <si>
+    <t>Serrano</t>
+  </si>
+  <si>
+    <t>Porro</t>
+  </si>
+  <si>
+    <t>Tuk</t>
+  </si>
+  <si>
+    <t>Data Addition</t>
   </si>
 </sst>
 </file>
@@ -150,9 +180,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -435,218 +471,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>101</v>
       </c>
-      <c r="D7">
-        <f>IF(C7&lt;&gt;"",C7,"")</f>
+      <c r="D8">
+        <f>IF(C8&lt;&gt;"",C8,"")</f>
         <v>101</v>
       </c>
-      <c r="F7">
-        <f>IF(D7&lt;&gt;"",D7,"")</f>
+      <c r="F8">
+        <f>IF(D8&lt;&gt;"",D8,"")</f>
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="G8">
+        <v>101</v>
+      </c>
+      <c r="I8">
+        <f>IF(G8&lt;&gt;"",G8,"")</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" ref="D8:D14" si="0">IF(C8&lt;&gt;"",C8,"")</f>
-        <v>Test TC-1</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" ref="F8:F14" si="1">IF(D8&lt;&gt;"",D8,"")</f>
-        <v>Test TC-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>Lorem Ipsun</v>
+        <f t="shared" ref="D9:D15" si="0">IF(C9&lt;&gt;"",C9,"")</f>
+        <v>Test TC-1</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="1"/>
-        <v>Lorem Ipsun</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" ref="F9:F15" si="1">IF(D9&lt;&gt;"",D9,"")</f>
+        <v>Test TC-1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" ref="I9:J15" si="2">IF(G9&lt;&gt;"",G9,"")</f>
+        <v>Test TC-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Test one</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>Test one</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="2"/>
+        <v>Test three</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>Max</v>
+        <v/>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
-        <v>Max</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>Mustermann</v>
+        <v>Max</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
+        <v>Max</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="2"/>
+        <v>Emiliy</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="2"/>
+        <v>Porro</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
         <v>Mustermann</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>Mustermann</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="2"/>
+        <v>Serrano</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="2"/>
+        <v>Tuk</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
         <v>0</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="G14">
+        <v>-20</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>71101</v>
-      </c>
-      <c r="D14">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>12345</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="0"/>
-        <v>71101</v>
-      </c>
-      <c r="F14">
+        <v>12345</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="1"/>
-        <v>71101</v>
+        <v>12345</v>
+      </c>
+      <c r="G15">
+        <v>98765</v>
+      </c>
+      <c r="H15">
+        <v>45562</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>98765</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>45562</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add more test cases and adjust data elements descriptions
</commit_message>
<xml_diff>
--- a/src/resources/TestData.xlsx
+++ b/src/resources/TestData.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
-  <si>
-    <t>Old ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Request Name</t>
   </si>
@@ -139,6 +136,18 @@
   </si>
   <si>
     <t>Data Addition</t>
+  </si>
+  <si>
+    <t>TC-4</t>
+  </si>
+  <si>
+    <t>Put Comment</t>
+  </si>
+  <si>
+    <t>Test four</t>
+  </si>
+  <si>
+    <t>Post ID</t>
   </si>
 </sst>
 </file>
@@ -471,102 +480,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
       </c>
       <c r="C8">
         <v>101</v>
@@ -586,16 +611,23 @@
         <f>IF(G8&lt;&gt;"",G8,"")</f>
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>102</v>
+      </c>
+      <c r="L8">
+        <f>IF(K8&lt;&gt;"",K8,"")</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" ref="D9:D15" si="0">IF(C9&lt;&gt;"",C9,"")</f>
@@ -606,22 +638,26 @@
         <v>Test TC-1</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" ref="I9:J15" si="2">IF(G9&lt;&gt;"",G9,"")</f>
         <v>Test TC-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L9" t="str">
+        <f t="shared" ref="L9:L10" si="3">IF(K9&lt;&gt;"",K9,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -632,16 +668,23 @@
         <v>Test one</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="2"/>
         <v>Test three</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="3"/>
+        <v>Test four</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -655,16 +698,20 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L11" t="str">
+        <f t="shared" ref="L11" si="4">IF(J11&lt;&gt;"",J11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -675,10 +722,10 @@
         <v>Max</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="2"/>
@@ -689,15 +736,15 @@
         <v>Porro</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -708,10 +755,10 @@
         <v>Mustermann</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="2"/>
@@ -722,12 +769,12 @@
         <v>Tuk</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -755,12 +802,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>12345</v>
@@ -789,7 +836,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>

</xml_diff>